<commit_message>
Adiciona arquivos com informações do plot do PLSR com filtro SG
</commit_message>
<xml_diff>
--- a/Partial Least Squares Regression/plot_infos_plsr_sg.xlsx
+++ b/Partial Least Squares Regression/plot_infos_plsr_sg.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,22 +446,22 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>R²</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>RMSE</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Offset</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>Slope</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Offset</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>RMSE</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>R²</t>
         </is>
       </c>
     </row>
@@ -477,16 +477,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.8468752211974486</v>
+        <v>0.8468752211974487</v>
       </c>
       <c r="D2" t="n">
-        <v>2.144096902730135</v>
+        <v>1.039782495631067</v>
       </c>
       <c r="E2" t="n">
-        <v>1.039782495631067</v>
+        <v>2.144096902730103</v>
       </c>
       <c r="F2" t="n">
-        <v>0.8468752211974486</v>
+        <v>0.8468752211974507</v>
       </c>
     </row>
     <row r="3">
@@ -501,40 +501,40 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.8085515093001355</v>
+        <v>0.7819065743440405</v>
       </c>
       <c r="D3" t="n">
-        <v>2.681170709591382</v>
+        <v>1.240912192912479</v>
       </c>
       <c r="E3" t="n">
-        <v>1.240912192912479</v>
+        <v>2.681170709591383</v>
       </c>
       <c r="F3" t="n">
-        <v>0.7819065743440404</v>
+        <v>0.8085515093001358</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>PH</t>
+          <t>SST</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Referência</t>
+          <t>Validação</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.7348983805227955</v>
+        <v>0.7193969855382728</v>
       </c>
       <c r="D4" t="n">
-        <v>0.8699332366140413</v>
+        <v>1.113369604707316</v>
       </c>
       <c r="E4" t="n">
-        <v>0.159078493150226</v>
+        <v>2.418510666719811</v>
       </c>
       <c r="F4" t="n">
-        <v>0.734898380522796</v>
+        <v>0.8260454883791656</v>
       </c>
     </row>
     <row r="5">
@@ -545,74 +545,74 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Predição</t>
+          <t>Referência</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.5405533510559278</v>
+        <v>0.7348983805227961</v>
       </c>
       <c r="D5" t="n">
-        <v>1.508740819072787</v>
+        <v>0.1590784931502259</v>
       </c>
       <c r="E5" t="n">
-        <v>0.2323240819676005</v>
+        <v>0.8699332366140435</v>
       </c>
       <c r="F5" t="n">
-        <v>0.4345712290132755</v>
+        <v>0.7348983805227949</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>AT</t>
+          <t>PH</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Referência</t>
+          <t>Predição</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.6086435674804007</v>
+        <v>0.4345712290132756</v>
       </c>
       <c r="D6" t="n">
-        <v>0.4390035190982435</v>
+        <v>0.2323240819676005</v>
       </c>
       <c r="E6" t="n">
-        <v>0.366979749761504</v>
+        <v>1.508740819072787</v>
       </c>
       <c r="F6" t="n">
-        <v>0.6086435674804005</v>
+        <v>0.5405533510559278</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>AT</t>
+          <t>PH</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Predição</t>
+          <t>Validação</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.5517827793060538</v>
+        <v>0.3946745576599974</v>
       </c>
       <c r="D7" t="n">
-        <v>0.5024077388366772</v>
+        <v>0.2036338527448653</v>
       </c>
       <c r="E7" t="n">
-        <v>0.4166389311005666</v>
+        <v>1.167112287674117</v>
       </c>
       <c r="F7" t="n">
-        <v>0.4955617936147404</v>
+        <v>0.6527151239015688</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>FIRMEZA (N)</t>
+          <t>AT</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -621,22 +621,22 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.6662668389410734</v>
+        <v>0.6086435674804005</v>
       </c>
       <c r="D8" t="n">
-        <v>171.2074248707973</v>
+        <v>0.366979749761504</v>
       </c>
       <c r="E8" t="n">
-        <v>59.37081403273279</v>
+        <v>0.4390035190982437</v>
       </c>
       <c r="F8" t="n">
-        <v>0.6662668389410731</v>
+        <v>0.6086435674804006</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>FIRMEZA (N)</t>
+          <t>AT</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -645,64 +645,184 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.5574744806366017</v>
+        <v>0.4955617936147407</v>
       </c>
       <c r="D9" t="n">
-        <v>227.0862397431741</v>
+        <v>0.4166389311005665</v>
       </c>
       <c r="E9" t="n">
-        <v>73.83410854066643</v>
+        <v>0.5024077388366772</v>
       </c>
       <c r="F9" t="n">
-        <v>0.4838601084893146</v>
+        <v>0.5517827793060537</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>UBS (%)</t>
+          <t>AT</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Referência</t>
+          <t>Validação</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.7658680342825452</v>
+        <v>0.6962065952275118</v>
       </c>
       <c r="D10" t="n">
-        <v>3.593486468355089</v>
+        <v>0.2408035552299508</v>
       </c>
       <c r="E10" t="n">
-        <v>1.556335544271717</v>
+        <v>0.01022350279104511</v>
       </c>
       <c r="F10" t="n">
-        <v>0.7658680342825455</v>
+        <v>0.972386623417224</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>FIRMEZA (N)</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Referência</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>0.6662668389410731</v>
+      </c>
+      <c r="D11" t="n">
+        <v>59.37081403273279</v>
+      </c>
+      <c r="E11" t="n">
+        <v>171.2074248707974</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.6662668389410729</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>FIRMEZA (N)</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Predição</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>0.4838601084893143</v>
+      </c>
+      <c r="D12" t="n">
+        <v>73.83410854066645</v>
+      </c>
+      <c r="E12" t="n">
+        <v>227.0862397431742</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.5574744806366013</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>FIRMEZA (N)</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Validação</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>0.4340161042135656</v>
+      </c>
+      <c r="D13" t="n">
+        <v>58.11770368330181</v>
+      </c>
+      <c r="E13" t="n">
+        <v>92.05045793939775</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.795228770311138</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
           <t>UBS (%)</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Referência</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>0.7658680342825456</v>
+      </c>
+      <c r="D14" t="n">
+        <v>1.556335544271717</v>
+      </c>
+      <c r="E14" t="n">
+        <v>3.593486468355088</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.7658680342825454</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>UBS (%)</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
         <is>
           <t>Predição</t>
         </is>
       </c>
-      <c r="C11" t="n">
-        <v>0.7271266460288287</v>
-      </c>
-      <c r="D11" t="n">
-        <v>4.146919951898043</v>
-      </c>
-      <c r="E11" t="n">
+      <c r="C15" t="n">
+        <v>0.6427565007783145</v>
+      </c>
+      <c r="D15" t="n">
         <v>1.922449975788665</v>
       </c>
-      <c r="F11" t="n">
-        <v>0.6427565007783147</v>
+      <c r="E15" t="n">
+        <v>4.146919951898045</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.7271266460288284</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>UBS (%)</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Validação</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>0.7298634450088908</v>
+      </c>
+      <c r="D16" t="n">
+        <v>1.126301319276778</v>
+      </c>
+      <c r="E16" t="n">
+        <v>3.445387826869926</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.7715225655986494</v>
       </c>
     </row>
   </sheetData>

</xml_diff>